<commit_message>
push 1 of 2
</commit_message>
<xml_diff>
--- a/updated names.xlsx
+++ b/updated names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjcar\Documents\GitHub\humanhelminths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16F0D98-105E-410A-A65E-CBE29770D652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F909247C-BF30-4299-8BCB-40D264A1D982}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="6863" xr2:uid="{81D29333-090C-48CE-9290-6777CE443D8F}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -737,7 +737,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2"/>
     </row>

</xml_diff>

<commit_message>
updated names push 2
all names now verified by colin
</commit_message>
<xml_diff>
--- a/updated names.xlsx
+++ b/updated names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjcar\Documents\GitHub\humanhelminths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F909247C-BF30-4299-8BCB-40D264A1D982}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2CD260-BC12-4F41-97F5-DA8AB6E4DB9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="6863" xr2:uid="{81D29333-090C-48CE-9290-6777CE443D8F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="81">
   <si>
     <t xml:space="preserve">Onchocerca dewittei </t>
   </si>
@@ -152,16 +152,127 @@
     <t>EYEBALL PARASITE https://www.cambridge.org/core/journals/journal-of-helminthology/article/first-instance-of-human-philophthalmosis-in-israel/BA2638FA6967565E995848A7C4E01736</t>
   </si>
   <si>
-    <t>Was this actually the name?</t>
-  </si>
-  <si>
-    <t>Filaria sanguinis (Thought to have been a threat in the late 1800s. Any follow-up on this?) Echinocactus hominis (All records from 1800s) Distomum rathouisi (Observed once in late 1800s - any more cases?) Cladorchis watsoni (One case reported in early 1900s) Cheilobus quadrilabiatus (Data on whether it infects humans seems inconclusive) Agamodistomum ophthalmobium (Really old records say it’s a parasite of the human eye?) Wuchereria lewisi (1969 man in Brazil - any follow up?) Trichobilharzia brevis (May cause dermatitis - Japan 1966) Pseudamphistomum aethiopicum (Infects humans “uncommonly” according to a book published in 2013) Mermis nigrescens (Weird case in an infant’s mouth - does this count?) Echinostoma japonica (In Korea?) Diorchitrema formosanus (Very very little info on this, but it’s listed as infecting humans in the Oxford textbook of medicine in 2003?) Centrocestus kurokawai (Journals/textbooks say yes but can’t find original source) Bunostomum trigonocephalum (Leaning toward yes, but can’t get a clear confirmation on this) Bertiella satyri (Also unclear, might be the same as B. studeri?)</t>
-  </si>
-  <si>
     <t xml:space="preserve">No </t>
   </si>
   <si>
     <t>I would include Trichobilharzia ocellata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filaria sanguinis </t>
+  </si>
+  <si>
+    <t>Thought to have been a threat in the late 1800s. Any follow-up on this?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Echinocactus hominis </t>
+  </si>
+  <si>
+    <t>All records from 1800s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Distomum rathouisi </t>
+  </si>
+  <si>
+    <t>Observed once in late 1800s - any more cases?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cladorchis watsoni </t>
+  </si>
+  <si>
+    <t>One case reported in early 1900s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheilobus quadrilabiatus </t>
+  </si>
+  <si>
+    <t>Data on whether it infects humans seems inconclusive)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agamodistomum ophthalmobium </t>
+  </si>
+  <si>
+    <t>Really old records say it’s a parasite of the human eye?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wuchereria lewisi </t>
+  </si>
+  <si>
+    <t>1969 man in Brazil - any follow up?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trichobilharzia brevis </t>
+  </si>
+  <si>
+    <t>May cause dermatitis - Japan 1966)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudamphistomum aethiopicum </t>
+  </si>
+  <si>
+    <t>Infects humans “uncommonly” according to a book published in 2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mermis nigrescens </t>
+  </si>
+  <si>
+    <t>Weird case in an infant’s mouth - does this count?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Echinostoma japonica </t>
+  </si>
+  <si>
+    <t>In Korea?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diorchitrema formosanus </t>
+  </si>
+  <si>
+    <t>Very very little info on this, but it’s listed as infecting humans in the Oxford textbook of medicine in 2003?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centrocestus kurokawai </t>
+  </si>
+  <si>
+    <t>Journals/textbooks say yes but can’t find original source)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bunostomum trigonocephalum </t>
+  </si>
+  <si>
+    <t>Leaning toward yes, but can’t get a clear confirmation on this)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertiella satyri </t>
+  </si>
+  <si>
+    <t>Also unclear, might be the same as B. studeri?)</t>
+  </si>
+  <si>
+    <t>Oof. Check this out: https://ac.els-cdn.com/S2052297518300763/1-s2.0-S2052297518300763-main.pdf?_tid=fe1d04ff-6175-4af7-b44a-7868f96f9353&amp;acdnat=1538660979_08bad23216f33360ab4f14119d32eaf9</t>
+  </si>
+  <si>
+    <t>I would just include Mansonella ozzardi and Mansonella perstans; perstans is the current name for Filaria sanguinis I think</t>
+  </si>
+  <si>
+    <t>Echinococcus hominis but still I think not a valid name</t>
+  </si>
+  <si>
+    <t>Just include Fasciolopsis buski</t>
+  </si>
+  <si>
+    <t>It's Alaria now but I say leave it out</t>
+  </si>
+  <si>
+    <t>I can't even find a good record of this</t>
+  </si>
+  <si>
+    <t>I don't think this is zoonotic in a meaningful way</t>
+  </si>
+  <si>
+    <t>RESURRECTION https://link.springer.com/article/10.1007/s00436-011-2300-0</t>
+  </si>
+  <si>
+    <t>Was this actually the name? I got nothing, feels like an autocorrect</t>
   </si>
 </sst>
 </file>
@@ -545,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566B9754-E51B-4025-9D98-EC463354161C}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -714,7 +825,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -747,25 +858,203 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>